<commit_message>
midplate 4 layers, chicker shell off limit switch idea
</commit_message>
<xml_diff>
--- a/Chicker/POWER_BOARD_BOM_JAN22.xlsx
+++ b/Chicker/POWER_BOARD_BOM_JAN22.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\henry\Documents\Documents\University\GitHub\The_Bots\Electrical\Chicker\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA2BF1A8-128A-4131-A368-7537C58D3C5B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FEF74D3-E88C-498A-BAB7-4594550DB3C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5112" yWindow="17172" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="POWER_BOARD" sheetId="1" r:id="rId1"/>
@@ -2180,8 +2180,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AF75"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" zoomScale="101" workbookViewId="0">
-      <selection activeCell="C57" sqref="C57"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="101" workbookViewId="0">
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
chicker discharge circuit finalized
</commit_message>
<xml_diff>
--- a/Chicker/POWER_BOARD_BOM_JAN22.xlsx
+++ b/Chicker/POWER_BOARD_BOM_JAN22.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\henry\Documents\Documents\University\GitHub\The_Bots\Electrical\Chicker\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FEF74D3-E88C-498A-BAB7-4594550DB3C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A24C1761-5AD1-495B-AA24-F35A0675B979}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5112" yWindow="17172" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -160,7 +160,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1070" uniqueCount="346">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1067" uniqueCount="347">
   <si>
     <t>Reference</t>
   </si>
@@ -1198,6 +1198,9 @@
   </si>
   <si>
     <t>&lt;- feeders loading fee 2.02 per component for standard (if we choose black it has to be standard not economic)</t>
+  </si>
+  <si>
+    <t>SMBJ5338B-TP</t>
   </si>
 </sst>
 </file>
@@ -2181,7 +2184,7 @@
   <dimension ref="A1:AF75"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" zoomScale="101" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+      <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3504,7 +3507,7 @@
         <v>59</v>
       </c>
       <c r="B18" t="s">
-        <v>60</v>
+        <v>346</v>
       </c>
       <c r="C18" t="s">
         <v>53</v>
@@ -3512,15 +3515,6 @@
       <c r="D18" t="s">
         <v>8</v>
       </c>
-      <c r="E18" t="s">
-        <v>61</v>
-      </c>
-      <c r="F18" t="s">
-        <v>236</v>
-      </c>
-      <c r="G18" t="s">
-        <v>296</v>
-      </c>
       <c r="H18">
         <v>0.47399999999999998</v>
       </c>
@@ -3536,7 +3530,7 @@
       </c>
       <c r="O18">
         <f t="shared" si="0"/>
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="P18">
         <f t="shared" si="5"/>
@@ -3552,7 +3546,7 @@
       </c>
       <c r="S18">
         <f t="shared" si="1"/>
-        <v>4.74</v>
+        <v>0</v>
       </c>
       <c r="T18">
         <f t="shared" si="8"/>

</xml_diff>

<commit_message>
chicker modifications (mostly ready to order)
</commit_message>
<xml_diff>
--- a/Chicker/POWER_BOARD_BOM_JAN22.xlsx
+++ b/Chicker/POWER_BOARD_BOM_JAN22.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\henry\Documents\Documents\University\GitHub\The_Bots\Electrical\Chicker\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9131F4C7-FB07-4868-A0F5-A35475901587}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D384094-DD55-4867-A39F-D7A770E2C0B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3396" yWindow="2244" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="768" yWindow="768" windowWidth="23040" windowHeight="12204" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="POWER_BOARD" sheetId="1" r:id="rId1"/>
@@ -160,7 +160,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1068" uniqueCount="350">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1069" uniqueCount="351">
   <si>
     <t>Reference</t>
   </si>
@@ -1210,6 +1210,9 @@
   </si>
   <si>
     <t>LMJ12MF1P0R008</t>
+  </si>
+  <si>
+    <t>&lt;- real total</t>
   </si>
 </sst>
 </file>
@@ -2196,10 +2199,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AG80"/>
+  <dimension ref="A1:AH80"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A61" zoomScale="101" workbookViewId="0">
-      <selection activeCell="A69" sqref="A69"/>
+    <sheetView tabSelected="1" topLeftCell="I49" zoomScale="101" workbookViewId="0">
+      <selection activeCell="AG69" sqref="AG69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -2212,11 +2215,11 @@
     <col min="7" max="7" width="16.5546875" customWidth="1"/>
     <col min="8" max="8" width="18.77734375" customWidth="1"/>
     <col min="9" max="11" width="8.88671875" customWidth="1"/>
-    <col min="12" max="12" width="12.21875" customWidth="1"/>
-    <col min="13" max="13" width="12.77734375" customWidth="1"/>
-    <col min="14" max="14" width="12.21875" customWidth="1"/>
-    <col min="15" max="17" width="17.21875" customWidth="1"/>
-    <col min="18" max="18" width="20.88671875" customWidth="1"/>
+    <col min="12" max="12" width="12.21875" hidden="1" customWidth="1"/>
+    <col min="13" max="13" width="12.77734375" hidden="1" customWidth="1"/>
+    <col min="14" max="14" width="12.21875" hidden="1" customWidth="1"/>
+    <col min="15" max="17" width="17.21875" hidden="1" customWidth="1"/>
+    <col min="18" max="18" width="20.88671875" hidden="1" customWidth="1"/>
     <col min="19" max="21" width="8.88671875" customWidth="1"/>
     <col min="22" max="22" width="10" customWidth="1"/>
     <col min="26" max="26" width="17.88671875" customWidth="1"/>
@@ -2224,6 +2227,7 @@
     <col min="29" max="29" width="12.6640625" customWidth="1"/>
     <col min="30" max="30" width="13.77734375" customWidth="1"/>
     <col min="32" max="32" width="12.88671875" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="13.21875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26">
@@ -5875,7 +5879,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="49" spans="1:32">
+    <row r="49" spans="1:34">
       <c r="A49" t="s">
         <v>147</v>
       </c>
@@ -5960,7 +5964,7 @@
       <c r="AC49" s="3"/>
       <c r="AF49" s="3"/>
     </row>
-    <row r="50" spans="1:32">
+    <row r="50" spans="1:34">
       <c r="A50" t="s">
         <v>150</v>
       </c>
@@ -6050,7 +6054,7 @@
         <v>10.78</v>
       </c>
     </row>
-    <row r="51" spans="1:32">
+    <row r="51" spans="1:34">
       <c r="A51" t="s">
         <v>152</v>
       </c>
@@ -6133,7 +6137,7 @@
         <v>2.02</v>
       </c>
     </row>
-    <row r="52" spans="1:32">
+    <row r="52" spans="1:34">
       <c r="A52" t="s">
         <v>155</v>
       </c>
@@ -6217,7 +6221,7 @@
         <v>69.260000000000005</v>
       </c>
     </row>
-    <row r="53" spans="1:32">
+    <row r="53" spans="1:34">
       <c r="A53" t="s">
         <v>157</v>
       </c>
@@ -6304,7 +6308,7 @@
         <v>30.96</v>
       </c>
     </row>
-    <row r="54" spans="1:32">
+    <row r="54" spans="1:34">
       <c r="A54" t="s">
         <v>160</v>
       </c>
@@ -6380,7 +6384,7 @@
       <c r="AC54" s="3"/>
       <c r="AF54" s="3"/>
     </row>
-    <row r="55" spans="1:32">
+    <row r="55" spans="1:34">
       <c r="A55" t="s">
         <v>164</v>
       </c>
@@ -6460,7 +6464,7 @@
         <v>5.3</v>
       </c>
     </row>
-    <row r="56" spans="1:32">
+    <row r="56" spans="1:34">
       <c r="A56" t="s">
         <v>168</v>
       </c>
@@ -6540,7 +6544,7 @@
         <v>0.57999999999999996</v>
       </c>
     </row>
-    <row r="57" spans="1:32">
+    <row r="57" spans="1:34">
       <c r="A57" t="s">
         <v>172</v>
       </c>
@@ -6623,7 +6627,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:32">
+    <row r="58" spans="1:34">
       <c r="A58" t="s">
         <v>176</v>
       </c>
@@ -6693,17 +6697,11 @@
       <c r="Y58">
         <v>7</v>
       </c>
-      <c r="AB58" t="s">
-        <v>273</v>
-      </c>
-      <c r="AC58" s="3">
-        <v>60.88</v>
-      </c>
-      <c r="AF58" s="3">
-        <v>60.88</v>
-      </c>
-    </row>
-    <row r="59" spans="1:32">
+      <c r="AG58">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="59" spans="1:34">
       <c r="A59" t="s">
         <v>179</v>
       </c>
@@ -6780,18 +6778,20 @@
         <v>10</v>
       </c>
       <c r="AB59" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="AC59" s="3">
-        <f>SUM(AC44:AC58)</f>
-        <v>291.61</v>
+        <v>60.88</v>
       </c>
       <c r="AF59" s="3">
-        <f>SUM(AF44:AF58)</f>
-        <v>229.42000000000004</v>
-      </c>
-    </row>
-    <row r="60" spans="1:32">
+        <v>60.88</v>
+      </c>
+      <c r="AG59">
+        <f>AG58+61.14</f>
+        <v>281.14</v>
+      </c>
+    </row>
+    <row r="60" spans="1:34">
       <c r="A60" t="s">
         <v>182</v>
       </c>
@@ -6871,18 +6871,22 @@
         <v>330</v>
       </c>
       <c r="AB60" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="AC60" s="3">
-        <f>0.12*AC59</f>
-        <v>34.993200000000002</v>
+        <f>SUM(AC44:AC59)</f>
+        <v>291.61</v>
       </c>
       <c r="AF60" s="3">
-        <f>0.12*AF59</f>
-        <v>27.530400000000004</v>
-      </c>
-    </row>
-    <row r="61" spans="1:32" s="8" customFormat="1">
+        <f>SUM(AF44:AF59)</f>
+        <v>229.42000000000004</v>
+      </c>
+      <c r="AG60" s="3">
+        <f>AG59</f>
+        <v>281.14</v>
+      </c>
+    </row>
+    <row r="61" spans="1:34" s="8" customFormat="1">
       <c r="A61" s="8" t="s">
         <v>185</v>
       </c>
@@ -6956,16 +6960,24 @@
         <v>1</v>
       </c>
       <c r="AB61" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="AC61" s="3">
-        <v>17.5</v>
-      </c>
+        <f>0.12*AC60</f>
+        <v>34.993200000000002</v>
+      </c>
+      <c r="AD61"/>
+      <c r="AE61"/>
       <c r="AF61" s="3">
-        <v>17.5</v>
-      </c>
-    </row>
-    <row r="62" spans="1:32">
+        <f>0.12*AF60</f>
+        <v>27.530400000000004</v>
+      </c>
+      <c r="AG61" s="3">
+        <f>0.12*AG60</f>
+        <v>33.736799999999995</v>
+      </c>
+    </row>
+    <row r="62" spans="1:34">
       <c r="A62" t="s">
         <v>187</v>
       </c>
@@ -7041,19 +7053,22 @@
       <c r="Z62" t="s">
         <v>332</v>
       </c>
-      <c r="AB62" s="8" t="s">
-        <v>265</v>
-      </c>
-      <c r="AC62" s="10">
-        <f>SUM(AC59:AC61)</f>
-        <v>344.10320000000002</v>
-      </c>
-      <c r="AF62" s="10">
-        <f>SUM(AF59:AF61)</f>
-        <v>274.45040000000006</v>
-      </c>
-    </row>
-    <row r="63" spans="1:32">
+      <c r="AB62" t="s">
+        <v>276</v>
+      </c>
+      <c r="AC62" s="3">
+        <v>17.5</v>
+      </c>
+      <c r="AD62" s="8"/>
+      <c r="AE62" s="8"/>
+      <c r="AF62" s="3">
+        <v>17.5</v>
+      </c>
+      <c r="AG62" s="3">
+        <v>17.5</v>
+      </c>
+    </row>
+    <row r="63" spans="1:34">
       <c r="A63" t="s">
         <v>189</v>
       </c>
@@ -7126,10 +7141,26 @@
       <c r="X63">
         <v>0</v>
       </c>
-      <c r="AC63" s="3"/>
-      <c r="AF63" s="3"/>
-    </row>
-    <row r="64" spans="1:32">
+      <c r="AB63" s="8" t="s">
+        <v>265</v>
+      </c>
+      <c r="AC63" s="10">
+        <f>SUM(AC60:AC62)</f>
+        <v>344.10320000000002</v>
+      </c>
+      <c r="AF63" s="10">
+        <f>SUM(AF60:AF62)</f>
+        <v>274.45040000000006</v>
+      </c>
+      <c r="AG63" s="10">
+        <f>SUM(AG60:AG62)</f>
+        <v>332.3768</v>
+      </c>
+      <c r="AH63" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="64" spans="1:34">
       <c r="A64" t="s">
         <v>193</v>
       </c>
@@ -7205,16 +7236,10 @@
       <c r="Y64">
         <v>20</v>
       </c>
-      <c r="AC64" s="3">
-        <f>AC62+$Z$70</f>
-        <v>564.2152000000001</v>
-      </c>
-      <c r="AF64" s="3">
-        <f>AF62+$Z$70</f>
-        <v>494.56240000000008</v>
-      </c>
-    </row>
-    <row r="65" spans="1:32" s="8" customFormat="1">
+      <c r="AC64" s="3"/>
+      <c r="AF64" s="3"/>
+    </row>
+    <row r="65" spans="1:33" s="8" customFormat="1">
       <c r="A65" s="8" t="s">
         <v>196</v>
       </c>
@@ -7290,19 +7315,23 @@
       <c r="Y65" s="8">
         <v>10</v>
       </c>
-      <c r="AB65" t="s">
-        <v>277</v>
-      </c>
+      <c r="AB65"/>
       <c r="AC65" s="3">
-        <f>AC64/10</f>
-        <v>56.421520000000008</v>
-      </c>
+        <f>AC63+$Z$70</f>
+        <v>564.2152000000001</v>
+      </c>
+      <c r="AD65"/>
+      <c r="AE65"/>
       <c r="AF65" s="3">
-        <f>AF64/10</f>
-        <v>49.456240000000008</v>
-      </c>
-    </row>
-    <row r="66" spans="1:32">
+        <f>AF63+$Z$70</f>
+        <v>494.56240000000008</v>
+      </c>
+      <c r="AG65" s="3">
+        <f>AG63+$Z$70</f>
+        <v>552.48880000000008</v>
+      </c>
+    </row>
+    <row r="66" spans="1:33">
       <c r="A66" t="s">
         <v>199</v>
       </c>
@@ -7382,10 +7411,25 @@
         <f>COUNTIF(W2:W66,"DIGIKEY")-5</f>
         <v>30</v>
       </c>
-      <c r="AB66" s="8"/>
-      <c r="AC66" s="8"/>
-    </row>
-    <row r="67" spans="1:32">
+      <c r="AB66" t="s">
+        <v>277</v>
+      </c>
+      <c r="AC66" s="3">
+        <f>AC65/10</f>
+        <v>56.421520000000008</v>
+      </c>
+      <c r="AD66" s="8"/>
+      <c r="AE66" s="8"/>
+      <c r="AF66" s="3">
+        <f>AF65/10</f>
+        <v>49.456240000000008</v>
+      </c>
+      <c r="AG66" s="3">
+        <f>AG65/10</f>
+        <v>55.248880000000007</v>
+      </c>
+    </row>
+    <row r="67" spans="1:33">
       <c r="A67" t="s">
         <v>333</v>
       </c>
@@ -7461,8 +7505,10 @@
       <c r="Y67">
         <v>30</v>
       </c>
-    </row>
-    <row r="69" spans="1:32">
+      <c r="AB67" s="8"/>
+      <c r="AC67" s="8"/>
+    </row>
+    <row r="69" spans="1:33">
       <c r="W69">
         <f>COUNTIF(W2:W66,"JLC")</f>
         <v>30</v>
@@ -7472,7 +7518,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="70" spans="1:32">
+    <row r="70" spans="1:33">
       <c r="T70" t="s">
         <v>265</v>
       </c>
@@ -7495,7 +7541,7 @@
         <v>168.03584000000006</v>
       </c>
     </row>
-    <row r="71" spans="1:32">
+    <row r="71" spans="1:33">
       <c r="T71" t="s">
         <v>266</v>
       </c>
@@ -7506,12 +7552,12 @@
         <v>325</v>
       </c>
     </row>
-    <row r="73" spans="1:32">
+    <row r="73" spans="1:33">
       <c r="W73" t="s">
         <v>327</v>
       </c>
     </row>
-    <row r="74" spans="1:32">
+    <row r="74" spans="1:33">
       <c r="V74">
         <f>V60+V56+V31++V4</f>
         <v>70.08</v>
@@ -7520,13 +7566,13 @@
         <v>320</v>
       </c>
     </row>
-    <row r="75" spans="1:32">
+    <row r="75" spans="1:33">
       <c r="Z75">
         <f>Z69/8</f>
         <v>38</v>
       </c>
     </row>
-    <row r="80" spans="1:32">
+    <row r="80" spans="1:33">
       <c r="X80">
         <f>30*2</f>
         <v>60</v>
@@ -7539,7 +7585,7 @@
       <formula>AND(T2-S2&lt;3,T2&gt;S2)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Z1 A1:Y40 W68 A42:Y67 A41:E41 G41:Y41">
+  <conditionalFormatting sqref="Z1 A1:Y40 A41:E41 G41:Y41 A42:Y67 W68">
     <cfRule type="expression" dxfId="3" priority="1">
       <formula>AND($W1="DIGIKEY",$V1&gt;0,$X1&gt;0)</formula>
     </cfRule>

</xml_diff>